<commit_message>
data integrity unit test and specification complete
</commit_message>
<xml_diff>
--- a/DataIntegrityAnalysis/Spec Examples.xlsx
+++ b/DataIntegrityAnalysis/Spec Examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Common Addition" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>